<commit_message>
New advice filled in.
</commit_message>
<xml_diff>
--- a/promiss.xlsx
+++ b/promiss.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MAMP\htdocs\PROMISS-interface\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51473065-BBCB-4FF1-BFE8-7858D78D3CF4}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="A" sheetId="1" r:id="rId1"/>
@@ -21,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="45">
   <si>
     <t>Persoon</t>
   </si>
@@ -59,9 +53,6 @@
     <t>Tussendoor avond</t>
   </si>
   <si>
-    <t>1 handje noten</t>
-  </si>
-  <si>
     <t>Persuasive strategy</t>
   </si>
   <si>
@@ -116,9 +107,6 @@
     <t>man</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
     <t>1 PROMISS diepvriesmaaltijd (indien geen diepvriesmaaltijd, eet gebruikelijke avondeten)</t>
   </si>
   <si>
@@ -128,9 +116,6 @@
     <t>1 schaaltje yoghurt/kwark/melk + 1 portie GOLEAN</t>
   </si>
   <si>
-    <t>2 boterhammen met hartig beleg (bijv. kaas/vleeswaar/vis/ei)</t>
-  </si>
-  <si>
     <t>B</t>
   </si>
   <si>
@@ -144,12 +129,34 @@
   </si>
   <si>
     <t>8:00</t>
+  </si>
+  <si>
+    <t>Romviel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 volkoren boterhammen, 2 porties eiwitrijk beleg, 200 ml sojamelk
+</t>
+  </si>
+  <si>
+    <t>1,5 maatschepje PROMISS eiwitpoeder, 30 gram ongezouten noten, 50 gram rauwkost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100 gram fruit of 2 blokjes pure chocolade </t>
+  </si>
+  <si>
+    <t xml:space="preserve">200 gram groente, 70 gram onbereid vlees of 50 gram onbereid vis of 100 gram onbereid vegetarisch product, 125 gram aardappelen of 75 gram rijst of 50 gram pasta </t>
+  </si>
+  <si>
+    <t>1,5 maatschepje PROMISS eiwitpoeder, 30 gram ongezouten noten</t>
+  </si>
+  <si>
+    <t>Griekse yoghurt 10%, 4 dadels, 4 lepels (50 gram) muesli, 200 ml sojamelk</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
@@ -257,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="justify"/>
@@ -324,6 +331,9 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="justify" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -631,18 +641,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -665,7 +675,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C2" s="5"/>
     </row>
@@ -674,33 +684,33 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:4" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="17"/>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>22</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="8"/>
     </row>
@@ -722,10 +732,10 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>6</v>
@@ -733,14 +743,12 @@
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>33</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="C11" s="13"/>
       <c r="D11" s="12"/>
     </row>
     <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -748,10 +756,10 @@
         <v>3</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="D12" s="12"/>
     </row>
@@ -760,10 +768,10 @@
         <v>7</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>9</v>
+        <v>27</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>43</v>
       </c>
       <c r="D13" s="12"/>
     </row>
@@ -772,10 +780,10 @@
         <v>4</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>35</v>
+        <v>26</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>39</v>
       </c>
       <c r="D14" s="12"/>
     </row>
@@ -784,13 +792,13 @@
         <v>8</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>9</v>
+        <v>25</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>40</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -798,10 +806,10 @@
         <v>10</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>32</v>
+        <v>24</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>42</v>
       </c>
       <c r="D16" s="13"/>
     </row>
@@ -810,10 +818,10 @@
         <v>11</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="D17" s="12"/>
     </row>
@@ -824,14 +832,14 @@
     </row>
     <row r="19" spans="1:4" s="11" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B19" s="16"/>
       <c r="C19" s="16"/>
     </row>
     <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B20" s="22"/>
       <c r="C20" s="15"/>
@@ -910,7 +918,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
@@ -936,7 +944,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C2" s="5"/>
     </row>
@@ -945,33 +953,33 @@
         <v>1</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:4" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="17"/>
     </row>
     <row r="5" spans="1:4" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>22</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="8"/>
     </row>
@@ -993,10 +1001,10 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>6</v>
@@ -1004,10 +1012,10 @@
     </row>
     <row r="11" spans="1:4" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>9</v>
@@ -1019,10 +1027,10 @@
         <v>3</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D12" s="12"/>
     </row>
@@ -1031,10 +1039,10 @@
         <v>7</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D13" s="12"/>
     </row>
@@ -1043,13 +1051,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1057,7 +1065,7 @@
         <v>8</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" s="13" t="s">
         <v>9</v>
@@ -1069,10 +1077,10 @@
         <v>10</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D16" s="13"/>
     </row>
@@ -1081,10 +1089,10 @@
         <v>11</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D17" s="12"/>
     </row>
@@ -1095,14 +1103,14 @@
     </row>
     <row r="19" spans="1:4" s="11" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B19" s="16"/>
       <c r="C19" s="16"/>
     </row>
     <row r="20" spans="1:4" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B20" s="22"/>
       <c r="C20" s="15"/>

</xml_diff>